<commit_message>
update document based changes
</commit_message>
<xml_diff>
--- a/db/dummy_data/itslabel/translations/ENGLISH_to_ARABIC.xlsx
+++ b/db/dummy_data/itslabel/translations/ENGLISH_to_ARABIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanoopsnair/Projects/itslabel.me/db/dummy_data/itslabel/translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5533AA-C9F1-D243-8CC2-38A66ECE18A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B77F46A-58D4-4D43-84FC-9613F9BE9460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="14600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="144">
   <si>
     <t>admin_user_email</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>نيكوتينات الألمنيوم</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -1289,15 +1292,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1319,8 +1322,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1527,7 +1533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1573,7 +1579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1596,7 +1602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1642,7 +1648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>

</xml_diff>